<commit_message>
maj paramètres de recherche 1e9bbc6276fbded24cd48b7b912d428638be2f1d
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/StructureDefinition-oncofair-medicationadministration-element.xlsx
+++ b/update-mapping-pn13/ig/StructureDefinition-oncofair-medicationadministration-element.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-01T09:30:15+00:00</t>
+    <t>2024-07-01T10:02:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -721,16 +721,16 @@
 </t>
   </si>
   <si>
+    <t>.inboundRelationship[typeCode=COMP].source[classCode=OBS, moodCode=EVN, code="type of medication usage"].value</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.category:code</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
     <t>codeElementAdministration</t>
-  </si>
-  <si>
-    <t>.inboundRelationship[typeCode=COMP].source[classCode=OBS, moodCode=EVN, code="type of medication usage"].value</t>
-  </si>
-  <si>
-    <t>MedicationAdministration.category:code</t>
-  </si>
-  <si>
-    <t>code</t>
   </si>
   <si>
     <t>MedicationAdministration.category:nature</t>
@@ -969,7 +969,7 @@
 </t>
   </si>
   <si>
-    <t>Actual start date and time of administration of the administration element</t>
+    <t>Effective date and time for startinf administration of the administration element</t>
   </si>
   <si>
     <t>The start of the period. The boundary is inclusive.</t>
@@ -4449,16 +4449,16 @@
         <v>101</v>
       </c>
       <c r="AK21" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL21" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AM21" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AN21" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AL21" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AM21" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>20</v>
@@ -4466,13 +4466,13 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B22" t="s" s="2">
         <v>217</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D22" t="s" s="2">
         <v>20</v>
@@ -4566,16 +4566,16 @@
         <v>101</v>
       </c>
       <c r="AK22" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AL22" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AM22" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AN22" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AL22" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AM22" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>20</v>
@@ -4692,7 +4692,7 @@
         <v>20</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>20</v>

</xml_diff>